<commit_message>
permisos y roles creado con migraciones y modelos
</commit_message>
<xml_diff>
--- a/utils/utilitario.xlsx
+++ b/utils/utilitario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="ScholarCampos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Tabla</t>
   </si>
@@ -79,6 +78,72 @@
   </si>
   <si>
     <t>codigo_nombres</t>
+  </si>
+  <si>
+    <t>permiso</t>
+  </si>
+  <si>
+    <t>modulo</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>porte</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>modulo_id</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>unsigned</t>
+  </si>
+  <si>
+    <t>modulos</t>
+  </si>
+  <si>
+    <t>foreign plural</t>
+  </si>
+  <si>
+    <t>permiso_id</t>
+  </si>
+  <si>
+    <t>permisos</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>usuarioRol</t>
+  </si>
+  <si>
+    <t>permisorol</t>
+  </si>
+  <si>
+    <t>rols</t>
+  </si>
+  <si>
+    <t>rol_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -94,12 +159,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,8 +185,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H9"/>
+  <dimension ref="C2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +493,7 @@
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -477,11 +551,11 @@
         <v>php artisan make:migration add__to_aula_table --table=aula</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G9" si="1">"php artisan make:model "&amp;PROPER(C4)&amp;" --migration"</f>
+        <f t="shared" ref="G4:G14" si="1">"php artisan make:model "&amp;PROPER(C4)&amp;" --migration"</f>
         <v>php artisan make:model Aula --migration</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H9" si="2">"php artisan make:controller "&amp;PROPER(C4)&amp;"Controller --resource"</f>
+        <f t="shared" ref="H4:H14" si="2">"php artisan make:controller "&amp;PROPER(C4)&amp;"Controller --resource"</f>
         <v>php artisan make:controller AulaController --resource</v>
       </c>
     </row>
@@ -579,6 +653,71 @@
       <c r="H9" t="str">
         <f t="shared" si="2"/>
         <v>php artisan make:controller CustodioController --resource</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>php artisan make:model Permiso --migration</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>php artisan make:controller PermisoController --resource</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>php artisan make:model Usuariorol --migration</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>php artisan make:controller UsuariorolController --resource</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>php artisan make:model Modulo --migration</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>php artisan make:controller ModuloController --resource</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>php artisan make:model Rol --migration</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>php artisan make:controller RolController --resource</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>php artisan make:model Permisorol --migration</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>php artisan make:controller PermisorolController --resource</v>
       </c>
     </row>
   </sheetData>
@@ -588,32 +727,407 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G2"/>
+  <dimension ref="C1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="1" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
         <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L9" si="0">"$table-&gt;"&amp;E4&amp;"('"&amp;D4&amp;"'"&amp;IF(LEN(F4)&gt;0,","&amp;F4&amp;"","")&amp;")"&amp;IF(H4&gt;0,"-&gt;nullable()","")&amp;IF(LEN(G4)&gt;0,"-&gt;default('"&amp;G4&amp;"')","")&amp;IF(LEN(I4)&gt;0,"-&gt;unsigned()","")&amp;";"&amp;IF(LEN(J4)&gt;0,"
+   $table-&gt;foreign('"&amp;D4&amp;"')-&gt;references('id')-&gt;on('"&amp;J4&amp;"');","")</f>
+        <v>$table-&gt;string('modulo',100);</v>
+      </c>
+      <c r="M4" t="str">
+        <f>"'"&amp;D4&amp;"',"</f>
+        <v>'modulo',</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;boolean('activo');</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ref="M5:M23" si="1">"'"&amp;D5&amp;"',"</f>
+        <v>'activo',</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('permiso',100);</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>'permiso',</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;integer('modulo_id')-&gt;unsigned();
+   $table-&gt;foreign('modulo_id')-&gt;references('id')-&gt;on('modulos');</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>'modulo_id',</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('descripcion',150);</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>'descripcion',</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L10" t="str">
+        <f t="shared" ref="L9:L23" si="2">"$table-&gt;"&amp;E10&amp;"('"&amp;D10&amp;"'"&amp;IF(LEN(F10)&gt;0,","&amp;F10&amp;"","")&amp;")"&amp;IF(H10&gt;0,"-&gt;nullable()","")&amp;IF(LEN(G10)&gt;0,"-&gt;default('"&amp;G10&amp;"')","")&amp;IF(LEN(I10)&gt;0,"-&gt;unsigned()","")&amp;";"&amp;IF(LEN(J10)&gt;0,"
+   $table-&gt;foreign('"&amp;D10&amp;"')-&gt;references('id')-&gt;on('"&amp;J10&amp;"');","")</f>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;integer('permiso_id')-&gt;unsigned();
+   $table-&gt;foreign('permiso_id')-&gt;references('id')-&gt;on('permisos');</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>'permiso_id',</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;integer('rol_id')-&gt;unsigned();
+   $table-&gt;foreign('rol_id')-&gt;references('id')-&gt;on('rols');</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>'rol_id',</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;string('rol',100);</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>'rol',</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>150</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;string('descripcion',150);</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>'descripcion',</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;integer('rol_id')-&gt;unsigned();
+   $table-&gt;foreign('rol_id')-&gt;references('id')-&gt;on('rols');</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>'rol_id',</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;integer('user_id')-&gt;unsigned();
+   $table-&gt;foreign('user_id')-&gt;references('id')-&gt;on('users');</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>'user_id',</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L23" t="str">
+        <f t="shared" si="2"/>
+        <v>$table-&gt;('');</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aumento de controlador y util de llenado de controlador
</commit_message>
<xml_diff>
--- a/utils/utilitario.xlsx
+++ b/utils/utilitario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Tabla</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>Controlador_codigo</t>
   </si>
 </sst>
 </file>
@@ -185,11 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +486,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H14"/>
+  <dimension ref="C2:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +503,7 @@
     <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>7</v>
       </c>
@@ -516,8 +522,11 @@
       <c r="H2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -537,8 +546,204 @@
         <f>"php artisan make:controller "&amp;PROPER(C3)&amp;"Controller --resource"</f>
         <v>php artisan make:controller CentroeducativoController --resource</v>
       </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="str">
+        <f>"&lt;?php
+namespace App\Http\Controllers;"&amp;"
+use App\Http\Requests;"&amp;"
+use App\Http\Controllers\Controller;"&amp;"
+use App\"&amp;PROPER(C3)&amp;";
+use Illuminate\Http\Request;"&amp;"
+use Session;"&amp;"
+class "&amp;PROPER(C3)&amp;"Controller extends Controller
+{
+    public function __construct()"&amp;"
+    {
+        $this-&gt;middleware('auth');"&amp;"
+        $this-&gt;middleware('authEmp:system');"&amp;"
+    }
+    /**
+     * Display a listing of the resource."&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function index()"&amp;"
+    {
+        $"&amp;(C3)&amp;" = "&amp;PROPER(C3)&amp;"::paginate(15);
+        return view('directory."&amp;(C3)&amp;".index', compact('"&amp;(C3)&amp;"'));
+    }
+    /**
+     * Show the form for creating a new resource."&amp;"
+     *
+     * @return Response
+     */
+    public function create()"&amp;"
+    {
+        return view('directory."&amp;(C3)&amp;".create');
+    }
+    /**
+     * Store a newly created resource in storage."&amp;"
+     *
+     * @return Response
+     */
+    public function store(Request $request)"&amp;"
+    {
+        "&amp;PROPER(C3)&amp;"::create($request-&gt;all());
+        Session::flash('flash_message', '¡"&amp;PROPER(C3)&amp;" añadido!');
+        return redirect('"&amp;(C3)&amp;"');
+    }
+    /**
+     * Display the specified resource."&amp;"
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)"&amp;"
+    {
+        $"&amp;(C3)&amp;" = "&amp;PROPER(C3)&amp;"::findOrFail($id);
+        return view('directory."&amp;(C3)&amp;".show', compact('"&amp;(C3)&amp;"'));
+    }
+    /**
+     * Show the form for editing the specified resource."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function edit($id)"&amp;"
+    {
+        $"&amp;(C3)&amp;" = "&amp;PROPER(C3)&amp;"::findOrFail($id);
+        return view('directory."&amp;(C3)&amp;".edit', compact('"&amp;(C3)&amp;"'));
+    }
+    /**
+     * Update the specified resource in storage."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)"&amp;"
+    {
+        $"&amp;(C3)&amp;" = "&amp;PROPER(C3)&amp;"::findOrFail($id);
+        $"&amp;(C3)&amp;"-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡"&amp;PROPER(C3)&amp;" actualizado!');
+        return redirect('"&amp;(C3)&amp;"');
+    }
+    /**
+     * Remove the specified resource from storage."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function destroy($id)"&amp;"
+    {
+        "&amp;PROPER(C3)&amp;"::destroy($id);
+        Session::flash('flash_message', '¡"&amp;PROPER(C3)&amp;" Borrado!');
+        return redirect('"&amp;(C3)&amp;"');
+    }"&amp;"
+}
+"</f>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Centroeducativo;
+use Illuminate\Http\Request;
+use Session;
+class CentroeducativoController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $centroeducativo = Centroeducativo::paginate(15);
+        return view('directory.centroeducativo.index', compact('centroeducativo'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.centroeducativo.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Centroeducativo::create($request-&gt;all());
+        Session::flash('flash_message', '¡Centroeducativo añadido!');
+        return redirect('centroeducativo');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $centroeducativo = Centroeducativo::findOrFail($id);
+        return view('directory.centroeducativo.show', compact('centroeducativo'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $centroeducativo = Centroeducativo::findOrFail($id);
+        return view('directory.centroeducativo.edit', compact('centroeducativo'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $centroeducativo = Centroeducativo::findOrFail($id);
+        $centroeducativo-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Centroeducativo actualizado!');
+        return redirect('centroeducativo');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Centroeducativo::destroy($id);
+        Session::flash('flash_message', '¡Centroeducativo Borrado!');
+        return redirect('centroeducativo');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -558,8 +763,204 @@
         <f t="shared" ref="H4:H14" si="2">"php artisan make:controller "&amp;PROPER(C4)&amp;"Controller --resource"</f>
         <v>php artisan make:controller AulaController --resource</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I14" si="3">"&lt;?php
+namespace App\Http\Controllers;"&amp;"
+use App\Http\Requests;"&amp;"
+use App\Http\Controllers\Controller;"&amp;"
+use App\"&amp;PROPER(C4)&amp;";
+use Illuminate\Http\Request;"&amp;"
+use Session;"&amp;"
+class "&amp;PROPER(C4)&amp;"Controller extends Controller
+{
+    public function __construct()"&amp;"
+    {
+        $this-&gt;middleware('auth');"&amp;"
+        $this-&gt;middleware('authEmp:system');"&amp;"
+    }
+    /**
+     * Display a listing of the resource."&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function index()"&amp;"
+    {
+        $"&amp;(C4)&amp;" = "&amp;PROPER(C4)&amp;"::paginate(15);
+        return view('directory."&amp;(C4)&amp;".index', compact('"&amp;(C4)&amp;"'));
+    }
+    /**
+     * Show the form for creating a new resource."&amp;"
+     *
+     * @return Response
+     */
+    public function create()"&amp;"
+    {
+        return view('directory."&amp;(C4)&amp;".create');
+    }
+    /**
+     * Store a newly created resource in storage."&amp;"
+     *
+     * @return Response
+     */
+    public function store(Request $request)"&amp;"
+    {
+        "&amp;PROPER(C4)&amp;"::create($request-&gt;all());
+        Session::flash('flash_message', '¡"&amp;PROPER(C4)&amp;" añadido!');
+        return redirect('"&amp;(C4)&amp;"');
+    }
+    /**
+     * Display the specified resource."&amp;"
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)"&amp;"
+    {
+        $"&amp;(C4)&amp;" = "&amp;PROPER(C4)&amp;"::findOrFail($id);
+        return view('directory."&amp;(C4)&amp;".show', compact('"&amp;(C4)&amp;"'));
+    }
+    /**
+     * Show the form for editing the specified resource."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function edit($id)"&amp;"
+    {
+        $"&amp;(C4)&amp;" = "&amp;PROPER(C4)&amp;"::findOrFail($id);
+        return view('directory."&amp;(C4)&amp;".edit', compact('"&amp;(C4)&amp;"'));
+    }
+    /**
+     * Update the specified resource in storage."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)"&amp;"
+    {
+        $"&amp;(C4)&amp;" = "&amp;PROPER(C4)&amp;"::findOrFail($id);
+        $"&amp;(C4)&amp;"-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡"&amp;PROPER(C4)&amp;" actualizado!');
+        return redirect('"&amp;(C4)&amp;"');
+    }
+    /**
+     * Remove the specified resource from storage."&amp;"
+     *
+     * @param  int  $id"&amp;"
+     *
+     * @return Response"&amp;"
+     */
+    public function destroy($id)"&amp;"
+    {
+        "&amp;PROPER(C4)&amp;"::destroy($id);
+        Session::flash('flash_message', '¡"&amp;PROPER(C4)&amp;" Borrado!');
+        return redirect('"&amp;(C4)&amp;"');
+    }"&amp;"
+}
+"</f>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Aula;
+use Illuminate\Http\Request;
+use Session;
+class AulaController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $aula = Aula::paginate(15);
+        return view('directory.aula.index', compact('aula'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.aula.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Aula::create($request-&gt;all());
+        Session::flash('flash_message', '¡Aula añadido!');
+        return redirect('aula');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $aula = Aula::findOrFail($id);
+        return view('directory.aula.show', compact('aula'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $aula = Aula::findOrFail($id);
+        return view('directory.aula.edit', compact('aula'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $aula = Aula::findOrFail($id);
+        $aula-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Aula actualizado!');
+        return redirect('aula');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Aula::destroy($id);
+        Session::flash('flash_message', '¡Aula Borrado!');
+        return redirect('aula');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -579,8 +980,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller TipoaulaController --resource</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Tipoaula;
+use Illuminate\Http\Request;
+use Session;
+class TipoaulaController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $tipoaula = Tipoaula::paginate(15);
+        return view('directory.tipoaula.index', compact('tipoaula'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.tipoaula.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Tipoaula::create($request-&gt;all());
+        Session::flash('flash_message', '¡Tipoaula añadido!');
+        return redirect('tipoaula');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $tipoaula = Tipoaula::findOrFail($id);
+        return view('directory.tipoaula.show', compact('tipoaula'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $tipoaula = Tipoaula::findOrFail($id);
+        return view('directory.tipoaula.edit', compact('tipoaula'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $tipoaula = Tipoaula::findOrFail($id);
+        $tipoaula-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Tipoaula actualizado!');
+        return redirect('tipoaula');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Tipoaula::destroy($id);
+        Session::flash('flash_message', '¡Tipoaula Borrado!');
+        return redirect('tipoaula');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -596,8 +1097,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller EstudianteController --resource</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Estudiante;
+use Illuminate\Http\Request;
+use Session;
+class EstudianteController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $estudiante = Estudiante::paginate(15);
+        return view('directory.estudiante.index', compact('estudiante'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.estudiante.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Estudiante::create($request-&gt;all());
+        Session::flash('flash_message', '¡Estudiante añadido!');
+        return redirect('estudiante');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $estudiante = Estudiante::findOrFail($id);
+        return view('directory.estudiante.show', compact('estudiante'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $estudiante = Estudiante::findOrFail($id);
+        return view('directory.estudiante.edit', compact('estudiante'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $estudiante = Estudiante::findOrFail($id);
+        $estudiante-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Estudiante actualizado!');
+        return redirect('estudiante');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Estudiante::destroy($id);
+        Session::flash('flash_message', '¡Estudiante Borrado!');
+        return redirect('estudiante');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -617,8 +1218,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller GrupoestudianteController --resource</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Grupoestudiante;
+use Illuminate\Http\Request;
+use Session;
+class GrupoestudianteController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $grupoestudiante = Grupoestudiante::paginate(15);
+        return view('directory.grupoestudiante.index', compact('grupoestudiante'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.grupoestudiante.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Grupoestudiante::create($request-&gt;all());
+        Session::flash('flash_message', '¡Grupoestudiante añadido!');
+        return redirect('grupoestudiante');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $grupoestudiante = Grupoestudiante::findOrFail($id);
+        return view('directory.grupoestudiante.show', compact('grupoestudiante'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $grupoestudiante = Grupoestudiante::findOrFail($id);
+        return view('directory.grupoestudiante.edit', compact('grupoestudiante'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $grupoestudiante = Grupoestudiante::findOrFail($id);
+        $grupoestudiante-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Grupoestudiante actualizado!');
+        return redirect('grupoestudiante');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Grupoestudiante::destroy($id);
+        Session::flash('flash_message', '¡Grupoestudiante Borrado!');
+        return redirect('grupoestudiante');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -634,8 +1335,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller ProfesorController --resource</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Profesor;
+use Illuminate\Http\Request;
+use Session;
+class ProfesorController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $profesor = Profesor::paginate(15);
+        return view('directory.profesor.index', compact('profesor'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.profesor.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Profesor::create($request-&gt;all());
+        Session::flash('flash_message', '¡Profesor añadido!');
+        return redirect('profesor');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $profesor = Profesor::findOrFail($id);
+        return view('directory.profesor.show', compact('profesor'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $profesor = Profesor::findOrFail($id);
+        return view('directory.profesor.edit', compact('profesor'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $profesor = Profesor::findOrFail($id);
+        $profesor-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Profesor actualizado!');
+        return redirect('profesor');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Profesor::destroy($id);
+        Session::flash('flash_message', '¡Profesor Borrado!');
+        return redirect('profesor');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>17</v>
       </c>
@@ -654,21 +1455,221 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller CustodioController --resource</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="I9" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Custodio;
+use Illuminate\Http\Request;
+use Session;
+class CustodioController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $custodio = Custodio::paginate(15);
+        return view('directory.custodio.index', compact('custodio'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.custodio.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Custodio::create($request-&gt;all());
+        Session::flash('flash_message', '¡Custodio añadido!');
+        return redirect('custodio');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $custodio = Custodio::findOrFail($id);
+        return view('directory.custodio.show', compact('custodio'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $custodio = Custodio::findOrFail($id);
+        return view('directory.custodio.edit', compact('custodio'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $custodio = Custodio::findOrFail($id);
+        $custodio-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Custodio actualizado!');
+        return redirect('custodio');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Custodio::destroy($id);
+        Session::flash('flash_message', '¡Custodio Borrado!');
+        return redirect('custodio');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>php artisan make:model Permiso --migration</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10" s="2" t="str">
         <f t="shared" si="2"/>
         <v>php artisan make:controller PermisoController --resource</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Permiso;
+use Illuminate\Http\Request;
+use Session;
+class PermisoController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $permiso = Permiso::paginate(15);
+        return view('directory.permiso.index', compact('permiso'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.permiso.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Permiso::create($request-&gt;all());
+        Session::flash('flash_message', '¡Permiso añadido!');
+        return redirect('permiso');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $permiso = Permiso::findOrFail($id);
+        return view('directory.permiso.show', compact('permiso'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $permiso = Permiso::findOrFail($id);
+        return view('directory.permiso.edit', compact('permiso'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $permiso = Permiso::findOrFail($id);
+        $permiso-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Permiso actualizado!');
+        return redirect('permiso');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Permiso::destroy($id);
+        Session::flash('flash_message', '¡Permiso Borrado!');
+        return redirect('permiso');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>36</v>
       </c>
@@ -680,8 +1681,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller UsuariorolController --resource</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Usuariorol;
+use Illuminate\Http\Request;
+use Session;
+class UsuariorolController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $usuarioRol = Usuariorol::paginate(15);
+        return view('directory.usuarioRol.index', compact('usuarioRol'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.usuarioRol.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Usuariorol::create($request-&gt;all());
+        Session::flash('flash_message', '¡Usuariorol añadido!');
+        return redirect('usuarioRol');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $usuarioRol = Usuariorol::findOrFail($id);
+        return view('directory.usuarioRol.show', compact('usuarioRol'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $usuarioRol = Usuariorol::findOrFail($id);
+        return view('directory.usuarioRol.edit', compact('usuarioRol'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $usuarioRol = Usuariorol::findOrFail($id);
+        $usuarioRol-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Usuariorol actualizado!');
+        return redirect('usuarioRol');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Usuariorol::destroy($id);
+        Session::flash('flash_message', '¡Usuariorol Borrado!');
+        return redirect('usuarioRol');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>20</v>
       </c>
@@ -693,8 +1794,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller ModuloController --resource</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Modulo;
+use Illuminate\Http\Request;
+use Session;
+class ModuloController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $modulo = Modulo::paginate(15);
+        return view('directory.modulo.index', compact('modulo'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.modulo.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Modulo::create($request-&gt;all());
+        Session::flash('flash_message', '¡Modulo añadido!');
+        return redirect('modulo');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $modulo = Modulo::findOrFail($id);
+        return view('directory.modulo.show', compact('modulo'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $modulo = Modulo::findOrFail($id);
+        return view('directory.modulo.edit', compact('modulo'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $modulo = Modulo::findOrFail($id);
+        $modulo-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Modulo actualizado!');
+        return redirect('modulo');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Modulo::destroy($id);
+        Session::flash('flash_message', '¡Modulo Borrado!');
+        return redirect('modulo');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>35</v>
       </c>
@@ -706,8 +1907,108 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller RolController --resource</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Rol;
+use Illuminate\Http\Request;
+use Session;
+class RolController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $rol = Rol::paginate(15);
+        return view('directory.rol.index', compact('rol'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.rol.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Rol::create($request-&gt;all());
+        Session::flash('flash_message', '¡Rol añadido!');
+        return redirect('rol');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $rol = Rol::findOrFail($id);
+        return view('directory.rol.show', compact('rol'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $rol = Rol::findOrFail($id);
+        return view('directory.rol.edit', compact('rol'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $rol = Rol::findOrFail($id);
+        $rol-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Rol actualizado!');
+        return redirect('rol');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Rol::destroy($id);
+        Session::flash('flash_message', '¡Rol Borrado!');
+        return redirect('rol');
+    }
+}
+</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -719,9 +2020,110 @@
         <f t="shared" si="2"/>
         <v>php artisan make:controller PermisorolController --resource</v>
       </c>
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&lt;?php
+namespace App\Http\Controllers;
+use App\Http\Requests;
+use App\Http\Controllers\Controller;
+use App\Permisorol;
+use Illuminate\Http\Request;
+use Session;
+class PermisorolController extends Controller
+{
+    public function __construct()
+    {
+        $this-&gt;middleware('auth');
+        $this-&gt;middleware('authEmp:system');
+    }
+    /**
+     * Display a listing of the resource.
+     *
+     * @return Response
+     */
+    public function index()
+    {
+        $permisorol = Permisorol::paginate(15);
+        return view('directory.permisorol.index', compact('permisorol'));
+    }
+    /**
+     * Show the form for creating a new resource.
+     *
+     * @return Response
+     */
+    public function create()
+    {
+        return view('directory.permisorol.create');
+    }
+    /**
+     * Store a newly created resource in storage.
+     *
+     * @return Response
+     */
+    public function store(Request $request)
+    {
+        Permisorol::create($request-&gt;all());
+        Session::flash('flash_message', '¡Permisorol añadido!');
+        return redirect('permisorol');
+    }
+    /**
+     * Display the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function show($id)
+    {
+        $permisorol = Permisorol::findOrFail($id);
+        return view('directory.permisorol.show', compact('permisorol'));
+    }
+    /**
+     * Show the form for editing the specified resource.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function edit($id)
+    {
+        $permisorol = Permisorol::findOrFail($id);
+        return view('directory.permisorol.edit', compact('permisorol'));
+    }
+    /**
+     * Update the specified resource in storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function update($id, Request $request)
+    {
+        $permisorol = Permisorol::findOrFail($id);
+        $permisorol-&gt;update($request-&gt;all());
+        Session::flash('flash_message', '¡Permisorol actualizado!');
+        return redirect('permisorol');
+    }
+    /**
+     * Remove the specified resource from storage.
+     *
+     * @param  int  $id
+     *
+     * @return Response
+     */
+    public function destroy($id)
+    {
+        Permisorol::destroy($id);
+        Session::flash('flash_message', '¡Permisorol Borrado!');
+        return redirect('permisorol');
+    }
+}
+</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -729,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +2301,7 @@
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L10" t="str">
-        <f t="shared" ref="L9:L23" si="2">"$table-&gt;"&amp;E10&amp;"('"&amp;D10&amp;"'"&amp;IF(LEN(F10)&gt;0,","&amp;F10&amp;"","")&amp;")"&amp;IF(H10&gt;0,"-&gt;nullable()","")&amp;IF(LEN(G10)&gt;0,"-&gt;default('"&amp;G10&amp;"')","")&amp;IF(LEN(I10)&gt;0,"-&gt;unsigned()","")&amp;";"&amp;IF(LEN(J10)&gt;0,"
+        <f t="shared" ref="L10:L23" si="2">"$table-&gt;"&amp;E10&amp;"('"&amp;D10&amp;"'"&amp;IF(LEN(F10)&gt;0,","&amp;F10&amp;"","")&amp;")"&amp;IF(H10&gt;0,"-&gt;nullable()","")&amp;IF(LEN(G10)&gt;0,"-&gt;default('"&amp;G10&amp;"')","")&amp;IF(LEN(I10)&gt;0,"-&gt;unsigned()","")&amp;";"&amp;IF(LEN(J10)&gt;0,"
    $table-&gt;foreign('"&amp;D10&amp;"')-&gt;references('id')-&gt;on('"&amp;J10&amp;"');","")</f>
         <v>$table-&gt;('');</v>
       </c>

</xml_diff>

<commit_message>
se aumenta seeder  de custodios
 arrancar asi:
`php artisan db:seed --class=ContactosTableSeeder`
</commit_message>
<xml_diff>
--- a/utils/utilitario.xlsx
+++ b/utils/utilitario.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
-    <sheet name="SchoolarModeloControlador" sheetId="2" r:id="rId2"/>
-    <sheet name="ScholarCampos" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="5" r:id="rId3"/>
+    <sheet name="SchoolarModeloControlador" sheetId="2" r:id="rId4"/>
+    <sheet name="ScholarCampos" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
   <si>
     <t>Tabla</t>
   </si>
@@ -147,19 +149,268 @@
   </si>
   <si>
     <t>Controlador_codigo</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>ciudad</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>documentoIdentificacion</t>
+  </si>
+  <si>
+    <t>cargo</t>
+  </si>
+  <si>
+    <t>compania</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>deleted_at</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>nombre_responsable</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>verification_token</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>"=&gt;"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>$faker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>name,</t>
+    </r>
+  </si>
+  <si>
+    <t>'Avianca Ec'</t>
+  </si>
+  <si>
+    <t>'Ecuador'</t>
+  </si>
+  <si>
+    <t>'QUITO'</t>
+  </si>
+  <si>
+    <t>'ACTIVO'</t>
+  </si>
+  <si>
+    <t>date($format = 'Y-m-d', $max = 'now')</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>$faker-&gt;</t>
+  </si>
+  <si>
+    <t>jobTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">randomNumber($nbDigits = NULL, $strict = false) </t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>companyEmail</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>remember_token</t>
+  </si>
+  <si>
+    <t>facebook_user_id</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>empresa</t>
+  </si>
+  <si>
+    <t>Admin System</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>$2y$10$Vso.J1tKkSIMJzx4SKu66ugXDrsvCfwzwrXHalUF0fe13bxaVWABC</t>
+  </si>
+  <si>
+    <t>$2y$10$9u7al21teXnMd/u8ZZ9oruyt/cYUc</t>
+  </si>
+  <si>
+    <t>$2y$10$TT4P87IOnWV7DEpUyrAg3O.8QJltyzI3Tw6XWZCU/aQkn/gklsbHK</t>
+  </si>
+  <si>
+    <t>Avianca EC</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <r>
+      <t>bcrypt(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'secret'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>system'</t>
+  </si>
+  <si>
+    <t>Avianca EC'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FF9876AA"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FFCC7832"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -188,12 +439,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,7 +481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -478,7 +747,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -486,21 +755,716 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="66.375" customWidth="1"/>
+    <col min="6" max="6" width="48.25" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f>"'"&amp;B5&amp;"' "&amp;"        "&amp;"=&gt;"&amp;D5&amp;E5&amp;","</f>
+        <v>'pais'         =&gt;'Ecuador',</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f t="shared" ref="F6:F16" si="0">"'"&amp;B6&amp;"' "&amp;"        "&amp;"=&gt;"&amp;D6&amp;E6&amp;","</f>
+        <v>'ciudad'         =&gt;'QUITO',</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'direccion'         =&gt;$faker-&gt;address,</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'documentoIdentificacion'         =&gt;$faker-&gt;randomNumber($nbDigits = NULL, $strict = false) ,</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'cargo'         =&gt;$faker-&gt;jobTitle,</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'compania'         =&gt;'Avianca Ec',</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'telefono'         =&gt;$faker-&gt;phoneNumber,</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'estado'         =&gt;'ACTIVO',</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'created_at'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'nombre_responsable'         =&gt;$faker-&gt;name,</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>''         =&gt;,</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'email'         =&gt;$faker-&gt;companyEmail,</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="4" t="str">
+        <f t="shared" ref="F23:F32" si="1">"'"&amp;B23&amp;"' "&amp;"        "&amp;"=&gt;"&amp;D23&amp;E23&amp;","</f>
+        <v>'name'         =&gt;$faker-&gt;name,</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'first_name'         =&gt;$faker-&gt;firstName,</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'last_name'         =&gt;$faker-&gt;lastName,</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'rol'         =&gt;system',</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'username'         =&gt;$faker-&gt;userName,</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'email'         =&gt;$faker-&gt;companyEmail,</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'password'         =&gt;bcrypt('secret'),</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'created_at'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'updated_at'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>'empresa'         =&gt;Avianca EC',</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="7">
+        <v>43316.792002314818</v>
+      </c>
+      <c r="K2" s="7">
+        <v>43316.792002314818</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="6" width="20.125" customWidth="1"/>
+    <col min="7" max="7" width="49.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
@@ -2127,7 +3091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M23"/>
   <sheetViews>
@@ -2135,11 +3099,11 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se crea seeders de proyectos y su logica inicial
</commit_message>
<xml_diff>
--- a/utils/utilitario.xlsx
+++ b/utils/utilitario.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="139">
   <si>
     <t>Tabla</t>
   </si>
@@ -335,9 +335,6 @@
     <t>check_list_id</t>
   </si>
   <si>
-    <t>imagen</t>
-  </si>
-  <si>
     <t>num_cajas</t>
   </si>
   <si>
@@ -350,12 +347,6 @@
     <t>codigo_barras</t>
   </si>
   <si>
-    <t>codigo_avianca</t>
-  </si>
-  <si>
-    <t>codigo_otro</t>
-  </si>
-  <si>
     <t>ip</t>
   </si>
   <si>
@@ -368,36 +359,6 @@
     <t>observaciones</t>
   </si>
   <si>
-    <t>codigo_contable</t>
-  </si>
-  <si>
-    <t>hp_warrantyLevel</t>
-  </si>
-  <si>
-    <t>hp_endDate</t>
-  </si>
-  <si>
-    <t>hp_displaySerialNumber</t>
-  </si>
-  <si>
-    <t>hp_modelNumber</t>
-  </si>
-  <si>
-    <t>hp_countryOfPurchase</t>
-  </si>
-  <si>
-    <t>hp_newProduct_seriesName</t>
-  </si>
-  <si>
-    <t>hp_newProduct_imageUrl</t>
-  </si>
-  <si>
-    <t>hp_warrantyResultRedirectUrl</t>
-  </si>
-  <si>
-    <t>empresa_procede1</t>
-  </si>
-  <si>
     <t>Avianca Ec</t>
   </si>
   <si>
@@ -417,24 +378,6 @@
   </si>
   <si>
     <t>MONITOR SN: CNC202S286</t>
-  </si>
-  <si>
-    <t>OW</t>
-  </si>
-  <si>
-    <t>A7H62LP</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>PC HP Compaq 6200 Pro con factor de forma reducido</t>
-  </si>
-  <si>
-    <t>https://ssl-product-images.www8-hp.com/digmedialib/prodimg/lowres/c02647335.jpg</t>
-  </si>
-  <si>
-    <t>/es-es/warrantyresult/hp-compaq-6200-pro-small-form-factor-pc/5037900/model/5037902?sku=A7H62LP</t>
   </si>
   <si>
     <t>function () {
@@ -461,13 +404,120 @@
   </si>
   <si>
     <t>randomElement($array = array ('SI', 'NO'))</t>
+  </si>
+  <si>
+    <t>no_orden</t>
+  </si>
+  <si>
+    <t>fecha_solicitud</t>
+  </si>
+  <si>
+    <t>fecha_ejecucion</t>
+  </si>
+  <si>
+    <t>hora_inicio</t>
+  </si>
+  <si>
+    <t>hora_fin</t>
+  </si>
+  <si>
+    <t>informe_manto_prev_cate_id</t>
+  </si>
+  <si>
+    <t>requerimiento</t>
+  </si>
+  <si>
+    <t>solucion</t>
+  </si>
+  <si>
+    <t>resolucion</t>
+  </si>
+  <si>
+    <t>vinculo</t>
+  </si>
+  <si>
+    <t>observacion</t>
+  </si>
+  <si>
+    <t>telefono_contacto</t>
+  </si>
+  <si>
+    <t>celular_contacto</t>
+  </si>
+  <si>
+    <t>email_contacto</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>publico_privado</t>
+  </si>
+  <si>
+    <t>Ayuda</t>
+  </si>
+  <si>
+    <t>blanco</t>
+  </si>
+  <si>
+    <t>publico</t>
+  </si>
+  <si>
+    <t>function () {
+            return App\Custodios::inRandomOrder()-&gt;first()-&gt;id;
+        }</t>
+  </si>
+  <si>
+    <t>time($format = 'H:i:s', $max = 'now')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sentence($nbWords = 6, $variableNbWords = true) </t>
+  </si>
+  <si>
+    <t>paragraph($nbSentences = 3, $variableNbSentences = true)</t>
+  </si>
+  <si>
+    <r>
+      <t>Uuid::</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FFFFC66D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>generate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>cellNumber</t>
+  </si>
+  <si>
+    <t>ipv4</t>
+  </si>
+  <si>
+    <t>randomElement($array = array ('blanco','like','unlike'))</t>
+  </si>
+  <si>
+    <t>randomElement($array = array ('publico','privado'))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +563,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FFFFC66D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -540,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -569,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K55"/>
+  <dimension ref="B2:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60:F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F40" s="4" t="str">
         <f t="shared" ref="F40:F55" si="2">"'"&amp;B40&amp;"' "&amp;"        "&amp;"=&gt;"&amp;D40&amp;E40&amp;","</f>
@@ -1463,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F41" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1480,7 +1540,7 @@
         <v>1039</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F42" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1497,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F43" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1514,7 +1574,7 @@
         <v>31</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F44" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1531,7 +1591,7 @@
         <v>1657</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F45" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1542,7 +1602,7 @@
     </row>
     <row r="46" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="4">
         <v>1</v>
@@ -1551,7 +1611,7 @@
         <v>65</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F46" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1560,10 +1620,10 @@
     </row>
     <row r="47" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>59</v>
@@ -1575,16 +1635,16 @@
     </row>
     <row r="48" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F48" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1593,14 +1653,14 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="F49" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1612,13 +1672,13 @@
         <v>34</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F50" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1627,7 +1687,7 @@
     </row>
     <row r="51" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C51" s="4"/>
       <c r="F51" s="4" t="str">
@@ -1640,13 +1700,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F52" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1655,16 +1715,16 @@
     </row>
     <row r="53" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E53" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F53" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1673,16 +1733,16 @@
     </row>
     <row r="54" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E54" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="F54" s="4" t="str">
         <f t="shared" si="2"/>
@@ -1691,20 +1751,360 @@
     </row>
     <row r="55" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E55" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F55" s="4" t="str">
         <f t="shared" si="2"/>
         <v>'observaciones'         =&gt;$faker-&gt;text,</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1047</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F60" s="4" t="str">
+        <f t="shared" ref="F60:F79" si="3">"'"&amp;B60&amp;"' "&amp;"        "&amp;"=&gt;"&amp;D60&amp;E60&amp;","</f>
+        <v>'custodio_id'         =&gt;function () {
+            return App\Custodios::inRandomOrder()-&gt;first()-&gt;id;
+        },</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="4">
+        <v>7</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F61" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'area_id'         =&gt;function () {
+            return App\User::inRandomOrder()-&gt;first()-&gt;id;
+        },</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="7">
+        <v>43411</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F62" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'fecha_solicitud'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="7">
+        <v>43411</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F63" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'fecha_ejecucion'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="11">
+        <v>0.87502314814814808</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'hora_inicio'         =&gt;$faker-&gt;time($format = 'H:i:s', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="11">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F65" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'hora_fin'         =&gt;$faker-&gt;time($format = 'H:i:s', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F66" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'informe_manto_prev_cate_id'         =&gt;function () {
+            return App\User::inRandomOrder()-&gt;first()-&gt;id;
+        },</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F67" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'requerimiento'         =&gt;$faker-&gt;sentence($nbWords = 6, $variableNbWords = true) ,</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F68" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'solucion'         =&gt;$faker-&gt;paragraph($nbSentences = 3, $variableNbSentences = true),</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F69" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'resolucion'         =&gt;$faker-&gt;paragraph($nbSentences = 3, $variableNbSentences = true),</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="7">
+        <v>43411.882314814815</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F70" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'created_at'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" s="7">
+        <v>43411.882314814815</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'updated_at'         =&gt;$faker-&gt;date($format = 'Y-m-d', $max = 'now'),</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="E72" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F72" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'vinculo'         =&gt;Uuid::generate(),</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'observacion'         =&gt;$faker-&gt;text,</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F74" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'telefono_contacto'         =&gt;$faker-&gt;phoneNumber,</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'celular_contacto'         =&gt;$faker-&gt;cellNumber,</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'email_contacto'         =&gt;$faker-&gt;companyEmail,</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F77" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'ip'         =&gt;$faker-&gt;ipv4,</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E78" t="s">
+        <v>137</v>
+      </c>
+      <c r="F78" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'like'         =&gt;randomElement($array = array ('blanco','like','unlike')),</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E79" t="s">
+        <v>138</v>
+      </c>
+      <c r="F79" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>'publico_privado'         =&gt;randomElement($array = array ('publico','privado')),</v>
       </c>
     </row>
   </sheetData>
@@ -1715,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AG4"/>
+      <selection activeCell="A5" sqref="A5:W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1763,189 +2163,199 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:33" ht="42.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="156.9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>702</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1039</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>31</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1657</v>
-      </c>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-      <c r="V4" s="7">
-        <v>43013.976990740739</v>
-      </c>
+      <c r="V4" s="7"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+    </row>
+    <row r="5" spans="1:33" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Z4" s="9">
-        <v>42096</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB4" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="M5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="Q5" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AG4" s="4"/>
+      <c r="R5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1047</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>43411</v>
+      </c>
+      <c r="F6" s="7">
+        <v>43411</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.87502314814814808</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="7">
+        <v>43411.882314814815</v>
+      </c>
+      <c r="N6" s="7">
+        <v>43411.882314814815</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>